<commit_message>
Add Lamp, Ceiling, floor
</commit_message>
<xml_diff>
--- a/Assets/Documents/ToDo.xlsx
+++ b/Assets/Documents/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Jams\TandemJam_1\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C818A0FE-CA2E-4320-BF84-D8BE38D3ECBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0DB38F-1229-4ADA-B5FE-30020CBC9BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8890" yWindow="460" windowWidth="28070" windowHeight="19610" xr2:uid="{6B6AB769-3234-4F83-9EFC-3B8AA71D9C63}"/>
+    <workbookView xWindow="57390" yWindow="100" windowWidth="19220" windowHeight="20470" xr2:uid="{6B6AB769-3234-4F83-9EFC-3B8AA71D9C63}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F7477E8-F995-4053-918D-5B2C3C009D15}">
   <dimension ref="B2:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="199" zoomScaleNormal="199" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -617,7 +617,7 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="1"/>
@@ -628,7 +628,7 @@
         <v>6</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="J8" t="s">
+      <c r="J8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="K8" s="1"/>
@@ -645,7 +645,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="J9" t="s">
+      <c r="J9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="K9" s="1"/>
@@ -668,7 +668,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="J11" t="s">
+      <c r="J11" s="4" t="s">
         <v>34</v>
       </c>
       <c r="K11" s="1"/>
@@ -682,7 +682,7 @@
         <v>18</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="J12" t="s">
+      <c r="J12" s="4" t="s">
         <v>35</v>
       </c>
       <c r="K12" s="1"/>
@@ -696,13 +696,13 @@
         <v>30</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="J13" t="s">
+      <c r="J13" s="4" t="s">
         <v>36</v>
       </c>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="1"/>
@@ -723,7 +723,7 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="1"/>
@@ -733,7 +733,7 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="4"/>

</xml_diff>